<commit_message>
update input inflow files
</commit_message>
<xml_diff>
--- a/Pittsboro_CC_DemandClassStats.xlsx
+++ b/Pittsboro_CC_DemandClassStats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dgorelic_ad_unc_edu/Documents/UNC/Research/WSC/Coding/WP/WaterPaths/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgorelic\OneDrive - University of North Carolina at Chapel Hill\UNC\Research\WSC\Coding\WP\WaterPaths\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="900" documentId="8_{C8E35AC9-AE47-4BC1-9B89-0F02DB53718A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2A21EA1F-2761-43C6-B4C3-AB0D10BA0615}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86269228-995F-4CCE-A765-45BC8EB19015}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{86269228-995F-4CCE-A765-45BC8EB19015}"/>
   </bookViews>
   <sheets>
     <sheet name="Pittsboro" sheetId="1" r:id="rId1"/>
@@ -2863,7 +2863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C932C3-199C-4AD4-8644-5C42E8B4AA28}">
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AB65" sqref="AB65"/>
     </sheetView>
   </sheetViews>
@@ -5212,7 +5212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B574F20-0A5F-4D69-9906-FFB905E30C7B}">
   <dimension ref="A1:AE88"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
@@ -7408,14 +7408,14 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DF1E017-875F-490E-A03E-5D51D72E6807}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8692fb02-64ee-477a-8829-0b8419474116"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8692fb02-64ee-477a-8829-0b8419474116"/>
     <ds:schemaRef ds:uri="e525f45e-12aa-43f1-99a0-18fd9df9a174"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>

</xml_diff>